<commit_message>
Fylt inn i P4
</commit_message>
<xml_diff>
--- a/Documents/test/Test - Fordeling av publikum.xlsx
+++ b/Documents/test/Test - Fordeling av publikum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mine Dokumenter\Skole\Høst 2015\Prosjekt\studentmatProsjekt\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mine Dokumenter\Skole\Høst 2015\Prosjekt\studentmatProsjekt\Documents\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -334,6 +334,132 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.3999076115485564E-2"/>
+                  <c:y val="9.9147366579177609E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-EB16-4F8B-89E1-44A62C50D39D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.488046194225722E-2"/>
+                  <c:y val="-0.10711909011373578"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-EB16-4F8B-89E1-44A62C50D39D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.4038635170603677E-2"/>
+                  <c:y val="0.12048993875765529"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-EB16-4F8B-89E1-44A62C50D39D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Ark2'!$A$2:$A$4</c:f>
@@ -1284,7 +1410,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>